<commit_message>
Finished the script and renamed it to Messages_Analysis
</commit_message>
<xml_diff>
--- a/DATA_ANALYSIS_CHECKLIST.xlsx
+++ b/DATA_ANALYSIS_CHECKLIST.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>Data Analysis - CHECKLIST</t>
   </si>
@@ -118,9 +117,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>NOK</t>
   </si>
   <si>
     <t>The average delivery delay time on the script is based on the messages that contain location (filter II). It should be based on all sent messages with delay.</t>
@@ -531,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,6 +592,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1066,7 @@
         <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="6:15" x14ac:dyDescent="0.25">
@@ -1156,6 +1153,7 @@
       <c r="J16" s="16" t="s">
         <v>30</v>
       </c>
+      <c r="O16" s="12"/>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" s="10">
@@ -1186,13 +1184,13 @@
         <v>2.1666666666666667E-2</v>
       </c>
       <c r="I18" s="19">
-        <v>1.2187500000000002E-2</v>
+        <v>2.1666666666666667E-2</v>
       </c>
       <c r="J18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
         <v>31</v>
-      </c>
-      <c r="K18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.25">
@@ -1206,13 +1204,13 @@
         <v>9.7569444444444448E-3</v>
       </c>
       <c r="I19" s="19">
-        <v>8.4375000000000006E-3</v>
+        <v>9.7569444444444448E-3</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="6:14" x14ac:dyDescent="0.25">
@@ -1226,13 +1224,13 @@
         <v>1.7187499999999998E-2</v>
       </c>
       <c r="I20" s="19">
-        <v>9.3749999999999997E-3</v>
+        <v>1.7187499999999998E-2</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="6:14" x14ac:dyDescent="0.25">
@@ -1243,10 +1241,10 @@
         <v>21</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>30</v>
@@ -1260,10 +1258,10 @@
         <v>22</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="16" t="s">
         <v>30</v>
@@ -1277,14 +1275,15 @@
         <v>23</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J23" s="16" t="s">
         <v>30</v>
       </c>
+      <c r="M23" s="30"/>
     </row>
     <row r="24" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F24" s="10">
@@ -1294,10 +1293,10 @@
         <v>24</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J24" s="16" t="s">
         <v>30</v>
@@ -1312,10 +1311,10 @@
         <v>25</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J25" s="16" t="s">
         <v>30</v>
@@ -1329,10 +1328,10 @@
         <v>26</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J26" s="16" t="s">
         <v>30</v>
@@ -1346,10 +1345,10 @@
         <v>27</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="J27" s="17" t="s">
         <v>30</v>

</xml_diff>